<commit_message>
Employee and Allowance Fix
</commit_message>
<xml_diff>
--- a/public/excel_files/masterlist-2014-12-10.xlsx
+++ b/public/excel_files/masterlist-2014-12-10.xlsx
@@ -16,12 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
   <si>
     <t>Payroll Period</t>
   </si>
   <si>
-    <t>2015-01-01-2015-01-15</t>
+    <t>2014-12-10-2014-12-25</t>
   </si>
   <si>
     <t>Payroll Date</t>
@@ -123,7 +123,10 @@
     <t>6,000.00</t>
   </si>
   <si>
-    <t>5,340.75</t>
+    <t>6,001.00</t>
+  </si>
+  <si>
+    <t>5,341.75</t>
   </si>
   <si>
     <t>HR Department</t>
@@ -1834,10 +1837,10 @@
         <v>30</v>
       </c>
       <c r="H8" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J8" s="9">
         <v>218</v>
@@ -1864,7 +1867,7 @@
         <v>391.25</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:1025" customHeight="1" ht="13.8">
@@ -3013,7 +3016,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -3112,16 +3115,16 @@
         <v>331</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F7" s="9">
         <v>500</v>
@@ -3133,7 +3136,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J7" s="9">
         <v>272.5</v>
@@ -3160,7 +3163,7 @@
         <v>752.63</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:1025" customHeight="1" ht="13.8">

</xml_diff>